<commit_message>
update rawdata for hait_ehfz
</commit_message>
<xml_diff>
--- a/data/output/posttrd_analysis.xlsx
+++ b/data/output/posttrd_analysis.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="50">
   <si>
     <t>DataDate</t>
   </si>
@@ -80,6 +80,15 @@
   </si>
   <si>
     <t>20210127</t>
+  </si>
+  <si>
+    <t>20210128</t>
+  </si>
+  <si>
+    <t>20210129</t>
+  </si>
+  <si>
+    <t>20210201</t>
   </si>
   <si>
     <t>8111_m_huat_9239</t>
@@ -515,7 +524,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J23"/>
+  <dimension ref="A1:J29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -558,10 +567,10 @@
         <v>10</v>
       </c>
       <c r="B2" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="C2" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="D2">
         <v>-201405.39</v>
@@ -590,10 +599,10 @@
         <v>11</v>
       </c>
       <c r="B3" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="C3" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="D3">
         <v>-4120</v>
@@ -622,10 +631,10 @@
         <v>12</v>
       </c>
       <c r="B4" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="C4" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="D4">
         <v>-5374.4</v>
@@ -654,10 +663,10 @@
         <v>13</v>
       </c>
       <c r="B5" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="C5" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="D5">
         <v>-1243.6</v>
@@ -686,10 +695,10 @@
         <v>14</v>
       </c>
       <c r="B6" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="C6" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="D6">
         <v>65510.1</v>
@@ -718,10 +727,10 @@
         <v>15</v>
       </c>
       <c r="B7" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="C7" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="D7">
         <v>-61522.6</v>
@@ -750,10 +759,10 @@
         <v>16</v>
       </c>
       <c r="B8" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="C8" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="D8">
         <v>-71421.8</v>
@@ -782,10 +791,10 @@
         <v>17</v>
       </c>
       <c r="B9" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="C9" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="D9">
         <v>-44586.1</v>
@@ -814,10 +823,10 @@
         <v>18</v>
       </c>
       <c r="B10" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="C10" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="D10">
         <v>60041.86</v>
@@ -846,10 +855,10 @@
         <v>19</v>
       </c>
       <c r="B11" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="C11" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="D11">
         <v>147494.95</v>
@@ -878,10 +887,10 @@
         <v>20</v>
       </c>
       <c r="B12" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="C12" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="D12">
         <v>-78605.7</v>
@@ -899,129 +908,129 @@
         <v>8957.049999999999</v>
       </c>
       <c r="I12">
-        <v>2148.93</v>
+        <v>1938.98</v>
       </c>
       <c r="J12">
-        <v>-43014.76</v>
+        <v>-42804.81</v>
       </c>
     </row>
     <row r="13" spans="1:10">
       <c r="A13" t="s">
-        <v>10</v>
+        <v>21</v>
       </c>
       <c r="B13" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="C13" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="D13">
-        <v>0.03</v>
+        <v>134156.92</v>
       </c>
       <c r="E13">
-        <v>0</v>
+        <v>-114465.2</v>
       </c>
       <c r="F13">
-        <v>0</v>
+        <v>-25.97</v>
       </c>
       <c r="G13">
-        <v>0.03</v>
+        <v>19665.75</v>
       </c>
       <c r="H13">
-        <v>0</v>
+        <v>8506.27</v>
       </c>
       <c r="I13">
-        <v>0</v>
+        <v>1988.22</v>
       </c>
       <c r="J13">
-        <v>0.03</v>
+        <v>9171.26</v>
       </c>
     </row>
     <row r="14" spans="1:10">
       <c r="A14" t="s">
-        <v>11</v>
+        <v>22</v>
       </c>
       <c r="B14" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="C14" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="D14">
-        <v>0</v>
+        <v>50751.9</v>
       </c>
       <c r="E14">
-        <v>1599.94</v>
+        <v>-190960</v>
       </c>
       <c r="F14">
-        <v>-3190</v>
+        <v>0</v>
       </c>
       <c r="G14">
-        <v>-1590.06</v>
+        <v>-140208.1</v>
       </c>
       <c r="H14">
-        <v>0</v>
+        <v>10185.62</v>
       </c>
       <c r="I14">
-        <v>0</v>
+        <v>2172.74</v>
       </c>
       <c r="J14">
-        <v>-1590.06</v>
+        <v>-152566.46</v>
       </c>
     </row>
     <row r="15" spans="1:10">
       <c r="A15" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="B15" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="C15" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="D15">
-        <v>0</v>
+        <v>-4981.7</v>
       </c>
       <c r="E15">
-        <v>1700.31</v>
+        <v>-18797.7</v>
       </c>
       <c r="F15">
-        <v>6380.35</v>
+        <v>232</v>
       </c>
       <c r="G15">
-        <v>8080.66</v>
+        <v>-23547.4</v>
       </c>
       <c r="H15">
-        <v>0</v>
+        <v>7075.04</v>
       </c>
       <c r="I15">
-        <v>0</v>
+        <v>3601.5</v>
       </c>
       <c r="J15">
-        <v>8080.66</v>
+        <v>-34223.94</v>
       </c>
     </row>
     <row r="16" spans="1:10">
       <c r="A16" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="B16" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="C16" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="D16">
-        <v>0</v>
+        <v>0.03</v>
       </c>
       <c r="E16">
-        <v>4700.28</v>
+        <v>0</v>
       </c>
       <c r="F16">
-        <v>-3480.4</v>
+        <v>0</v>
       </c>
       <c r="G16">
-        <v>1219.89</v>
+        <v>0.03</v>
       </c>
       <c r="H16">
         <v>0</v>
@@ -1030,30 +1039,30 @@
         <v>0</v>
       </c>
       <c r="J16">
-        <v>1219.89</v>
+        <v>0.03</v>
       </c>
     </row>
     <row r="17" spans="1:10">
       <c r="A17" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="B17" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="C17" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="D17">
-        <v>80</v>
+        <v>0</v>
       </c>
       <c r="E17">
-        <v>1500.02</v>
+        <v>1599.94</v>
       </c>
       <c r="F17">
-        <v>-1450.4</v>
+        <v>-3190</v>
       </c>
       <c r="G17">
-        <v>129.62</v>
+        <v>-1590.06</v>
       </c>
       <c r="H17">
         <v>0</v>
@@ -1062,30 +1071,30 @@
         <v>0</v>
       </c>
       <c r="J17">
-        <v>129.62</v>
+        <v>-1590.06</v>
       </c>
     </row>
     <row r="18" spans="1:10">
       <c r="A18" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="B18" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="C18" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="D18">
         <v>0</v>
       </c>
       <c r="E18">
-        <v>1200.08</v>
+        <v>1700.31</v>
       </c>
       <c r="F18">
-        <v>1260.57</v>
+        <v>6380.35</v>
       </c>
       <c r="G18">
-        <v>2460.65</v>
+        <v>8080.66</v>
       </c>
       <c r="H18">
         <v>0</v>
@@ -1094,30 +1103,30 @@
         <v>0</v>
       </c>
       <c r="J18">
-        <v>2460.65</v>
+        <v>8080.66</v>
       </c>
     </row>
     <row r="19" spans="1:10">
       <c r="A19" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="B19" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="C19" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="D19">
         <v>0</v>
       </c>
       <c r="E19">
-        <v>1200.05</v>
+        <v>4700.28</v>
       </c>
       <c r="F19">
-        <v>-630.3200000000001</v>
+        <v>-3480.4</v>
       </c>
       <c r="G19">
-        <v>569.73</v>
+        <v>1219.89</v>
       </c>
       <c r="H19">
         <v>0</v>
@@ -1126,30 +1135,30 @@
         <v>0</v>
       </c>
       <c r="J19">
-        <v>569.73</v>
+        <v>1219.89</v>
       </c>
     </row>
     <row r="20" spans="1:10">
       <c r="A20" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="B20" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="C20" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="D20">
-        <v>0</v>
+        <v>80</v>
       </c>
       <c r="E20">
-        <v>1200.18</v>
+        <v>1500.02</v>
       </c>
       <c r="F20">
-        <v>2311.31</v>
+        <v>-1450.4</v>
       </c>
       <c r="G20">
-        <v>3511.49</v>
+        <v>129.62</v>
       </c>
       <c r="H20">
         <v>0</v>
@@ -1158,30 +1167,30 @@
         <v>0</v>
       </c>
       <c r="J20">
-        <v>3511.49</v>
+        <v>129.62</v>
       </c>
     </row>
     <row r="21" spans="1:10">
       <c r="A21" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="B21" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="C21" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="D21">
         <v>0</v>
       </c>
       <c r="E21">
-        <v>3700</v>
+        <v>1200.08</v>
       </c>
       <c r="F21">
-        <v>-3151.97</v>
+        <v>1260.57</v>
       </c>
       <c r="G21">
-        <v>548.03</v>
+        <v>2460.65</v>
       </c>
       <c r="H21">
         <v>0</v>
@@ -1190,30 +1199,30 @@
         <v>0</v>
       </c>
       <c r="J21">
-        <v>548.03</v>
+        <v>2460.65</v>
       </c>
     </row>
     <row r="22" spans="1:10">
       <c r="A22" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="B22" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="C22" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="D22">
         <v>0</v>
       </c>
       <c r="E22">
-        <v>1300</v>
+        <v>1200.05</v>
       </c>
       <c r="F22">
-        <v>0</v>
+        <v>-630.3200000000001</v>
       </c>
       <c r="G22">
-        <v>1300</v>
+        <v>569.73</v>
       </c>
       <c r="H22">
         <v>0</v>
@@ -1222,39 +1231,231 @@
         <v>0</v>
       </c>
       <c r="J22">
-        <v>1300</v>
+        <v>569.73</v>
       </c>
     </row>
     <row r="23" spans="1:10">
       <c r="A23" t="s">
+        <v>17</v>
+      </c>
+      <c r="B23" t="s">
+        <v>24</v>
+      </c>
+      <c r="C23" t="s">
+        <v>26</v>
+      </c>
+      <c r="D23">
+        <v>0</v>
+      </c>
+      <c r="E23">
+        <v>1200.18</v>
+      </c>
+      <c r="F23">
+        <v>2311.31</v>
+      </c>
+      <c r="G23">
+        <v>3511.49</v>
+      </c>
+      <c r="H23">
+        <v>0</v>
+      </c>
+      <c r="I23">
+        <v>0</v>
+      </c>
+      <c r="J23">
+        <v>3511.49</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10">
+      <c r="A24" t="s">
+        <v>18</v>
+      </c>
+      <c r="B24" t="s">
+        <v>24</v>
+      </c>
+      <c r="C24" t="s">
+        <v>26</v>
+      </c>
+      <c r="D24">
+        <v>0</v>
+      </c>
+      <c r="E24">
+        <v>3700</v>
+      </c>
+      <c r="F24">
+        <v>-3151.97</v>
+      </c>
+      <c r="G24">
+        <v>548.03</v>
+      </c>
+      <c r="H24">
+        <v>0</v>
+      </c>
+      <c r="I24">
+        <v>0</v>
+      </c>
+      <c r="J24">
+        <v>548.03</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10">
+      <c r="A25" t="s">
+        <v>19</v>
+      </c>
+      <c r="B25" t="s">
+        <v>24</v>
+      </c>
+      <c r="C25" t="s">
+        <v>26</v>
+      </c>
+      <c r="D25">
+        <v>0</v>
+      </c>
+      <c r="E25">
+        <v>1300</v>
+      </c>
+      <c r="F25">
+        <v>0</v>
+      </c>
+      <c r="G25">
+        <v>1300</v>
+      </c>
+      <c r="H25">
+        <v>0</v>
+      </c>
+      <c r="I25">
+        <v>0</v>
+      </c>
+      <c r="J25">
+        <v>1300</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10">
+      <c r="A26" t="s">
         <v>20</v>
       </c>
-      <c r="B23" t="s">
+      <c r="B26" t="s">
+        <v>24</v>
+      </c>
+      <c r="C26" t="s">
+        <v>26</v>
+      </c>
+      <c r="D26">
+        <v>0</v>
+      </c>
+      <c r="E26">
+        <v>1299.99</v>
+      </c>
+      <c r="F26">
+        <v>-210.18</v>
+      </c>
+      <c r="G26">
+        <v>1089.81</v>
+      </c>
+      <c r="H26">
+        <v>0</v>
+      </c>
+      <c r="I26">
+        <v>0</v>
+      </c>
+      <c r="J26">
+        <v>1089.81</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10">
+      <c r="A27" t="s">
         <v>21</v>
       </c>
-      <c r="C23" t="s">
+      <c r="B27" t="s">
+        <v>24</v>
+      </c>
+      <c r="C27" t="s">
+        <v>26</v>
+      </c>
+      <c r="D27">
+        <v>0</v>
+      </c>
+      <c r="E27">
+        <v>1299.91</v>
+      </c>
+      <c r="F27">
+        <v>-1261.16</v>
+      </c>
+      <c r="G27">
+        <v>38.74</v>
+      </c>
+      <c r="H27">
+        <v>0</v>
+      </c>
+      <c r="I27">
+        <v>0</v>
+      </c>
+      <c r="J27">
+        <v>38.74</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10">
+      <c r="A28" t="s">
+        <v>22</v>
+      </c>
+      <c r="B28" t="s">
+        <v>24</v>
+      </c>
+      <c r="C28" t="s">
+        <v>26</v>
+      </c>
+      <c r="D28">
+        <v>0</v>
+      </c>
+      <c r="E28">
+        <v>1300.07</v>
+      </c>
+      <c r="F28">
+        <v>2522.48</v>
+      </c>
+      <c r="G28">
+        <v>3822.55</v>
+      </c>
+      <c r="H28">
+        <v>0</v>
+      </c>
+      <c r="I28">
+        <v>0</v>
+      </c>
+      <c r="J28">
+        <v>3822.55</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10">
+      <c r="A29" t="s">
         <v>23</v>
       </c>
-      <c r="D23">
-        <v>0</v>
-      </c>
-      <c r="E23">
-        <v>1299.99</v>
-      </c>
-      <c r="F23">
-        <v>-210.18</v>
-      </c>
-      <c r="G23">
-        <v>1089.81</v>
-      </c>
-      <c r="H23">
-        <v>0</v>
-      </c>
-      <c r="I23">
-        <v>0</v>
-      </c>
-      <c r="J23">
-        <v>1089.81</v>
+      <c r="B29" t="s">
+        <v>24</v>
+      </c>
+      <c r="C29" t="s">
+        <v>26</v>
+      </c>
+      <c r="D29">
+        <v>-360</v>
+      </c>
+      <c r="E29">
+        <v>5699.83</v>
+      </c>
+      <c r="F29">
+        <v>-2384.16</v>
+      </c>
+      <c r="G29">
+        <v>2955.67</v>
+      </c>
+      <c r="H29">
+        <v>0</v>
+      </c>
+      <c r="I29">
+        <v>0</v>
+      </c>
+      <c r="J29">
+        <v>2955.67</v>
       </c>
     </row>
   </sheetData>
@@ -1264,7 +1465,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G12"/>
+  <dimension ref="A1:G15"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1287,10 +1488,10 @@
         <v>8</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
     </row>
     <row r="2" spans="1:7">
@@ -1298,7 +1499,7 @@
         <v>10</v>
       </c>
       <c r="B2" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="C2">
         <v>-201315.35</v>
@@ -1318,7 +1519,7 @@
         <v>11</v>
       </c>
       <c r="B3" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="C3">
         <v>-8390.059999999999</v>
@@ -1333,7 +1534,7 @@
         <v>-8906.700000000001</v>
       </c>
       <c r="G3" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
     </row>
     <row r="4" spans="1:7">
@@ -1341,7 +1542,7 @@
         <v>12</v>
       </c>
       <c r="B4" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="C4">
         <v>16545.16</v>
@@ -1364,7 +1565,7 @@
         <v>13</v>
       </c>
       <c r="B5" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="C5">
         <v>9756.889999999999</v>
@@ -1387,7 +1588,7 @@
         <v>14</v>
       </c>
       <c r="B6" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="C6">
         <v>-37416.28</v>
@@ -1410,7 +1611,7 @@
         <v>15</v>
       </c>
       <c r="B7" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="C7">
         <v>14116.85</v>
@@ -1433,7 +1634,7 @@
         <v>16</v>
       </c>
       <c r="B8" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="C8">
         <v>29972.23</v>
@@ -1456,7 +1657,7 @@
         <v>17</v>
       </c>
       <c r="B9" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="C9">
         <v>18658.39</v>
@@ -1479,7 +1680,7 @@
         <v>18</v>
       </c>
       <c r="B10" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="C10">
         <v>44436.79</v>
@@ -1502,7 +1703,7 @@
         <v>19</v>
       </c>
       <c r="B11" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="C11">
         <v>-45983.17</v>
@@ -1525,7 +1726,7 @@
         <v>20</v>
       </c>
       <c r="B12" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="C12">
         <v>-30818.97</v>
@@ -1534,13 +1735,82 @@
         <v>8957.049999999999</v>
       </c>
       <c r="E12">
-        <v>2148.93</v>
+        <v>1938.98</v>
       </c>
       <c r="F12">
-        <v>-41924.95</v>
+        <v>-41715</v>
       </c>
       <c r="G12">
         <v>2.700000002980232</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7">
+      <c r="A13" t="s">
+        <v>21</v>
+      </c>
+      <c r="B13" t="s">
+        <v>24</v>
+      </c>
+      <c r="C13">
+        <v>19704.49</v>
+      </c>
+      <c r="D13">
+        <v>8506.27</v>
+      </c>
+      <c r="E13">
+        <v>1988.22</v>
+      </c>
+      <c r="F13">
+        <v>9210</v>
+      </c>
+      <c r="G13">
+        <v>1.400000002235174</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7">
+      <c r="A14" t="s">
+        <v>22</v>
+      </c>
+      <c r="B14" t="s">
+        <v>24</v>
+      </c>
+      <c r="C14">
+        <v>-136385.55</v>
+      </c>
+      <c r="D14">
+        <v>10185.62</v>
+      </c>
+      <c r="E14">
+        <v>2172.74</v>
+      </c>
+      <c r="F14">
+        <v>-148743.91</v>
+      </c>
+      <c r="G14">
+        <v>2.900000004097819</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7">
+      <c r="A15" t="s">
+        <v>23</v>
+      </c>
+      <c r="B15" t="s">
+        <v>24</v>
+      </c>
+      <c r="C15">
+        <v>-20591.73</v>
+      </c>
+      <c r="D15">
+        <v>7075.04</v>
+      </c>
+      <c r="E15">
+        <v>3601.5</v>
+      </c>
+      <c r="F15">
+        <v>-31268.27</v>
+      </c>
+      <c r="G15">
+        <v>-2.400000006891787</v>
       </c>
     </row>
   </sheetData>
@@ -1550,7 +1820,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H11"/>
+  <dimension ref="A1:H14"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1564,22 +1834,22 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
     </row>
     <row r="2" spans="1:8">
@@ -1587,7 +1857,7 @@
         <v>11</v>
       </c>
       <c r="B2" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="C2">
         <v>979679.03</v>
@@ -1613,7 +1883,7 @@
         <v>12</v>
       </c>
       <c r="B3" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="C3">
         <v>987439.3</v>
@@ -1639,7 +1909,7 @@
         <v>13</v>
       </c>
       <c r="B4" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="C4">
         <v>994174.52</v>
@@ -1665,7 +1935,7 @@
         <v>14</v>
       </c>
       <c r="B5" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="C5">
         <v>8952815.75</v>
@@ -1691,7 +1961,7 @@
         <v>15</v>
       </c>
       <c r="B6" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="C6">
         <v>8959921.41</v>
@@ -1717,7 +1987,7 @@
         <v>16</v>
       </c>
       <c r="B7" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="C7">
         <v>8983563.08</v>
@@ -1743,7 +2013,7 @@
         <v>17</v>
       </c>
       <c r="B8" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="C8">
         <v>8992134.029999999</v>
@@ -1769,7 +2039,7 @@
         <v>18</v>
       </c>
       <c r="B9" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="C9">
         <v>8812476.859999999</v>
@@ -1795,7 +2065,7 @@
         <v>19</v>
       </c>
       <c r="B10" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="C10">
         <v>8970946.630000001</v>
@@ -1821,7 +2091,7 @@
         <v>20</v>
       </c>
       <c r="B11" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="C11">
         <v>8929799.67</v>
@@ -1840,6 +2110,84 @@
       </c>
       <c r="H11">
         <v>37128047.62</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8">
+      <c r="A12" t="s">
+        <v>21</v>
+      </c>
+      <c r="B12" t="s">
+        <v>24</v>
+      </c>
+      <c r="C12">
+        <v>8940500.029999999</v>
+      </c>
+      <c r="D12">
+        <v>8941580.68</v>
+      </c>
+      <c r="E12">
+        <v>28729111.64</v>
+      </c>
+      <c r="F12">
+        <v>7742209.07</v>
+      </c>
+      <c r="G12">
+        <v>29928483.25</v>
+      </c>
+      <c r="H12">
+        <v>37670692.32</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8">
+      <c r="A13" t="s">
+        <v>22</v>
+      </c>
+      <c r="B13" t="s">
+        <v>24</v>
+      </c>
+      <c r="C13">
+        <v>6615.32</v>
+      </c>
+      <c r="D13">
+        <v>6615.32</v>
+      </c>
+      <c r="E13">
+        <v>35782003.1</v>
+      </c>
+      <c r="F13">
+        <v>6009037.99</v>
+      </c>
+      <c r="G13">
+        <v>29779580.43</v>
+      </c>
+      <c r="H13">
+        <v>35788618.42</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8">
+      <c r="A14" t="s">
+        <v>23</v>
+      </c>
+      <c r="B14" t="s">
+        <v>24</v>
+      </c>
+      <c r="C14">
+        <v>5952465.72</v>
+      </c>
+      <c r="D14">
+        <v>5952465.72</v>
+      </c>
+      <c r="E14">
+        <v>29448287.77</v>
+      </c>
+      <c r="F14">
+        <v>5652274.89</v>
+      </c>
+      <c r="G14">
+        <v>29748478.6</v>
+      </c>
+      <c r="H14">
+        <v>35400753.49</v>
       </c>
     </row>
   </sheetData>
@@ -1849,7 +2197,7 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:Q11"/>
+  <dimension ref="A1:Q14"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1866,46 +2214,46 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="Q1" s="1" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
     </row>
     <row r="2" spans="1:17">
@@ -1913,10 +2261,10 @@
         <v>11</v>
       </c>
       <c r="B2" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="C2" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="D2">
         <v>519480</v>
@@ -1966,10 +2314,10 @@
         <v>12</v>
       </c>
       <c r="B3" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="C3" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="D3">
         <v>835626</v>
@@ -2019,10 +2367,10 @@
         <v>13</v>
       </c>
       <c r="B4" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="C4" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="D4">
         <v>2641173</v>
@@ -2072,10 +2420,10 @@
         <v>14</v>
       </c>
       <c r="B5" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="C5" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="D5">
         <v>4881789</v>
@@ -2125,10 +2473,10 @@
         <v>15</v>
       </c>
       <c r="B6" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="C6" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="D6">
         <v>7137006</v>
@@ -2178,10 +2526,10 @@
         <v>16</v>
       </c>
       <c r="B7" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="C7" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="D7">
         <v>8987127</v>
@@ -2231,10 +2579,10 @@
         <v>17</v>
       </c>
       <c r="B8" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="C8" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="D8">
         <v>10170823.5</v>
@@ -2284,10 +2632,10 @@
         <v>18</v>
       </c>
       <c r="B9" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="C9" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="D9">
         <v>10051660.59</v>
@@ -2317,7 +2665,7 @@
         <v>13617456.54</v>
       </c>
       <c r="M9">
-        <v>7809768</v>
+        <v>7354119</v>
       </c>
       <c r="N9">
         <v>0.96</v>
@@ -2329,7 +2677,7 @@
         <v>0.23</v>
       </c>
       <c r="Q9">
-        <v>0.86</v>
+        <v>0.91</v>
       </c>
     </row>
     <row r="10" spans="1:17">
@@ -2337,10 +2685,10 @@
         <v>19</v>
       </c>
       <c r="B10" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="C10" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="D10">
         <v>9707852.07</v>
@@ -2390,10 +2738,10 @@
         <v>20</v>
       </c>
       <c r="B11" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="C11" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="D11">
         <v>10767642</v>
@@ -2411,13 +2759,13 @@
         <v>126</v>
       </c>
       <c r="I11">
-        <v>7179058.140000001</v>
+        <v>7179058.14</v>
       </c>
       <c r="J11">
         <v>7178428</v>
       </c>
       <c r="K11">
-        <v>630.140000000596</v>
+        <v>630.1399999996647</v>
       </c>
       <c r="L11">
         <v>14357486.14</v>
@@ -2436,6 +2784,165 @@
       </c>
       <c r="Q11">
         <v>0.83</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17">
+      <c r="A12" t="s">
+        <v>21</v>
+      </c>
+      <c r="B12" t="s">
+        <v>24</v>
+      </c>
+      <c r="C12" t="s">
+        <v>25</v>
+      </c>
+      <c r="D12">
+        <v>10520512.5</v>
+      </c>
+      <c r="E12">
+        <v>13275142.49</v>
+      </c>
+      <c r="F12">
+        <v>42</v>
+      </c>
+      <c r="G12">
+        <v>47</v>
+      </c>
+      <c r="H12">
+        <v>174</v>
+      </c>
+      <c r="I12">
+        <v>7013675</v>
+      </c>
+      <c r="J12">
+        <v>7013675</v>
+      </c>
+      <c r="K12">
+        <v>0</v>
+      </c>
+      <c r="L12">
+        <v>14027350</v>
+      </c>
+      <c r="M12">
+        <v>9504177</v>
+      </c>
+      <c r="N12">
+        <v>0.95</v>
+      </c>
+      <c r="O12">
+        <v>0.89</v>
+      </c>
+      <c r="P12">
+        <v>0.27</v>
+      </c>
+      <c r="Q12">
+        <v>0.74</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17">
+      <c r="A13" t="s">
+        <v>22</v>
+      </c>
+      <c r="B13" t="s">
+        <v>24</v>
+      </c>
+      <c r="C13" t="s">
+        <v>25</v>
+      </c>
+      <c r="D13">
+        <v>8964265.5</v>
+      </c>
+      <c r="E13">
+        <v>16026007</v>
+      </c>
+      <c r="F13">
+        <v>41</v>
+      </c>
+      <c r="G13">
+        <v>48</v>
+      </c>
+      <c r="H13">
+        <v>170</v>
+      </c>
+      <c r="I13">
+        <v>5978513</v>
+      </c>
+      <c r="J13">
+        <v>5976177</v>
+      </c>
+      <c r="K13">
+        <v>2336</v>
+      </c>
+      <c r="L13">
+        <v>11954690</v>
+      </c>
+      <c r="M13">
+        <v>9150084</v>
+      </c>
+      <c r="N13">
+        <v>1.34</v>
+      </c>
+      <c r="O13">
+        <v>0.85</v>
+      </c>
+      <c r="P13">
+        <v>0.28</v>
+      </c>
+      <c r="Q13">
+        <v>0.65</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17">
+      <c r="A14" t="s">
+        <v>23</v>
+      </c>
+      <c r="B14" t="s">
+        <v>24</v>
+      </c>
+      <c r="C14" t="s">
+        <v>25</v>
+      </c>
+      <c r="D14">
+        <v>8426592</v>
+      </c>
+      <c r="E14">
+        <v>11089459</v>
+      </c>
+      <c r="F14">
+        <v>39</v>
+      </c>
+      <c r="G14">
+        <v>48</v>
+      </c>
+      <c r="H14">
+        <v>205</v>
+      </c>
+      <c r="I14">
+        <v>5641302</v>
+      </c>
+      <c r="J14">
+        <v>5617728</v>
+      </c>
+      <c r="K14">
+        <v>23574</v>
+      </c>
+      <c r="L14">
+        <v>11259030</v>
+      </c>
+      <c r="M14">
+        <v>7231003</v>
+      </c>
+      <c r="N14">
+        <v>0.98</v>
+      </c>
+      <c r="O14">
+        <v>0.8100000000000001</v>
+      </c>
+      <c r="P14">
+        <v>0.23</v>
+      </c>
+      <c r="Q14">
+        <v>0.78</v>
       </c>
     </row>
   </sheetData>

</xml_diff>